<commit_message>
solucion de busqueda por fecha sin datos
</commit_message>
<xml_diff>
--- a/Autoservicio_Correa/Casos de prueba.xlsx
+++ b/Autoservicio_Correa/Casos de prueba.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="78">
   <si>
     <t>Nombre del Proyecto</t>
   </si>
@@ -209,6 +209,66 @@
   </si>
   <si>
     <t>Al seleccionar Salir se cierra la sesión con el mensaje correspondiente</t>
+  </si>
+  <si>
+    <t>1 - Nuevo cliente que ingresa a la página</t>
+  </si>
+  <si>
+    <t>2 - Permisos y funciones de superusuario (staff)</t>
+  </si>
+  <si>
+    <t>Iniciar con superuser</t>
+  </si>
+  <si>
+    <t>Al iniciar con superuser deberá poder la opción de Cargar Promociones, Ver Pedidos y Buscar Pedidos.</t>
+  </si>
+  <si>
+    <t>Ingresa con superuser y se ven las solapas correspondientes. Todas funcionan.</t>
+  </si>
+  <si>
+    <t>Cargar promoción</t>
+  </si>
+  <si>
+    <t>El superuser podrá cargar una nueva promoción ingresando todos los datos correspondientes. Aquí podrá seleccionar una imagen de su equipo que acompañará a la promoción. Al finalizar lo dirigirá a la pantalla de inicio.</t>
+  </si>
+  <si>
+    <t>Permite cargar promoción, seleccionar imagen y se guarda todo en la base de datos. Redirige a la página de inicio.</t>
+  </si>
+  <si>
+    <t>Cargar promoción sin imagen</t>
+  </si>
+  <si>
+    <t>Si no hay una foto específica par subir con la promoción, el superuser no cargará ninguna pero el sitio le devolverá una imagen predefinida.</t>
+  </si>
+  <si>
+    <t>Permite cargar promoción sin subir una imagen, y al consultar la promoción se aprecia la imagen genérica.</t>
+  </si>
+  <si>
+    <t>Ver / Editar / Eliminar Promociones</t>
+  </si>
+  <si>
+    <t>Solo los superuser podrán editar o eliminar promociones. Lo podrán hacer desde la vista Leer Promociones con los botones específicos. Al editar y guardar los cambios lo redirigirá nuevamente a la vista de promociones. Si presiona eliminar, primero mostrará un mensaje para confirmar y una vez confirmada volverá a la vista de promociones.</t>
+  </si>
+  <si>
+    <t>Al ingresar a la vista de promociones se ven los botones correspondientes. Al editar abre formulario en edición y permite cambiar todos los datos (menos eliminar la foto), al guardar regresa a la vista anterior. Si presiono eliminar muestra el mensaje de confirmación y luego deconfirmar vuelve a la vista anterior donde ya no se muestra la promoción eliminada.</t>
+  </si>
+  <si>
+    <t>Ver todos los pedidos</t>
+  </si>
+  <si>
+    <t>Buscar pedidos</t>
+  </si>
+  <si>
+    <t>El superuser podrá ver todos los pedidos ingresados (de todos los clientes). Podrá ver el detalle y editarlos (no podrá eliminarlos). Luego de cada una de estas tareas regresará a la vista de pedidos. Los pedidos deberán estar ordenados por fecha de entrega, mostrando en la parte inferior los pedidos con entrega más vieja.</t>
+  </si>
+  <si>
+    <t>Con el superuser se muestra todos los pedidos de la base, se pueden ver en detalle y editar correctamente. Se aprecia la necesidad de mejorar esta funcionalidad limitando los permisos de clientes y superuser (estará disponible en versión 2.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El superuser podrá ingresar un fecha de entrega para ver solo los pedidos de dicha fecha. Al presionar buscar devolverá listado de los pedidos y podrá verlos o editarlos. Sin no hay pedidos, mostrata una mensaje indicándolo. </t>
+  </si>
+  <si>
+    <t>Busca correctamente los pedidos por fecha, en caso que no haya devuelve mensaje en pantalla.</t>
   </si>
 </sst>
 </file>
@@ -601,8 +661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,8 +695,8 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7">
-        <v>1</v>
+      <c r="B2" s="7" t="s">
+        <v>58</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="1" t="s">
@@ -959,8 +1019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -993,8 +1053,8 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7">
-        <v>2</v>
+      <c r="B2" s="7" t="s">
+        <v>59</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="1" t="s">
@@ -1065,13 +1125,13 @@
         <v>45109</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>15</v>
@@ -1085,13 +1145,13 @@
         <v>45109</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>15</v>
@@ -1105,13 +1165,13 @@
         <v>45109</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>15</v>
@@ -1125,19 +1185,19 @@
         <v>45109</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>5</v>
       </c>
@@ -1145,19 +1205,19 @@
         <v>45109</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>29</v>
+        <v>75</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>6</v>
       </c>
@@ -1165,13 +1225,13 @@
         <v>45109</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>33</v>
+        <v>77</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Listos los casos de prueba, falta el readme
</commit_message>
<xml_diff>
--- a/Autoservicio_Correa/Casos de prueba.xlsx
+++ b/Autoservicio_Correa/Casos de prueba.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="81">
   <si>
     <t>Nombre del Proyecto</t>
   </si>
@@ -265,10 +265,19 @@
     <t>Con el superuser se muestra todos los pedidos de la base, se pueden ver en detalle y editar correctamente. Se aprecia la necesidad de mejorar esta funcionalidad limitando los permisos de clientes y superuser (estará disponible en versión 2.0)</t>
   </si>
   <si>
-    <t xml:space="preserve">El superuser podrá ingresar un fecha de entrega para ver solo los pedidos de dicha fecha. Al presionar buscar devolverá listado de los pedidos y podrá verlos o editarlos. Sin no hay pedidos, mostrata una mensaje indicándolo. </t>
-  </si>
-  <si>
-    <t>Busca correctamente los pedidos por fecha, en caso que no haya devuelve mensaje en pantalla.</t>
+    <t>El superuser podrá ingresar un fecha de entrega para ver solo los pedidos de dicha fecha. Al presionar buscar devolverá listado de los pedidos y podrá verlos o editarlos. Sin no hay pedidos, mostrara una mensaje indicándolo. Si no carga fecha y presiona buscar, tambien devuelve mensaje.</t>
+  </si>
+  <si>
+    <t>Busca correctamente los pedidos por fecha, en caso que no haya devuelve mensaje en pantalla. Busco sin cargar fecha y tambien aparece pantalla con mensaje aclaratorio.</t>
+  </si>
+  <si>
+    <t>Eliminar superuser</t>
+  </si>
+  <si>
+    <t>Estará bloqueda la eliminación del superuser desde el sitio. Solamente desde el admin será posible.</t>
+  </si>
+  <si>
+    <t>Al ingresar a editar el perfil no se muestra la opción para eliminarlo.</t>
   </si>
 </sst>
 </file>
@@ -1019,8 +1028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1217,7 +1226,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>6</v>
       </c>
@@ -1237,7 +1246,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>7</v>
       </c>
@@ -1245,117 +1254,57 @@
         <v>45109</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>35</v>
+        <v>79</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>36</v>
+        <v>80</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>8</v>
-      </c>
-      <c r="B14" s="4">
-        <v>45109</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <v>9</v>
-      </c>
-      <c r="B15" s="4">
-        <v>45109</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="150" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>10</v>
-      </c>
-      <c r="B16" s="4">
-        <v>45109</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="150" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>11</v>
-      </c>
-      <c r="B17" s="4">
-        <v>45109</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>12</v>
-      </c>
-      <c r="B18" s="4">
-        <v>45109</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>15</v>
-      </c>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>